<commit_message>
Update live bets summary data
</commit_message>
<xml_diff>
--- a/live_bets_summary.xlsx
+++ b/live_bets_summary.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1439"/>
+  <dimension ref="A1:O1444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -82878,6 +82878,285 @@
       </c>
       <c r="O1439" t="n">
         <v>0.76</v>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="n">
+        <v>1.253911665</v>
+      </c>
+      <c r="B1440" t="n">
+        <v>79846027</v>
+      </c>
+      <c r="C1440" t="n">
+        <v>418201531416</v>
+      </c>
+      <c r="D1440" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="E1440" t="inlineStr">
+        <is>
+          <t>12:56</t>
+        </is>
+      </c>
+      <c r="F1440" t="inlineStr">
+        <is>
+          <t>SHEPPARTON</t>
+        </is>
+      </c>
+      <c r="G1440" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="H1440" t="inlineStr">
+        <is>
+          <t>SHREKS BROTHER</t>
+        </is>
+      </c>
+      <c r="I1440" t="inlineStr">
+        <is>
+          <t>LAY</t>
+        </is>
+      </c>
+      <c r="J1440" t="inlineStr">
+        <is>
+          <t>UNMATCHED</t>
+        </is>
+      </c>
+      <c r="K1440" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="L1440" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="M1440" t="inlineStr"/>
+      <c r="N1440" t="inlineStr">
+        <is>
+          <t>ACTIVE</t>
+        </is>
+      </c>
+      <c r="O1440" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="n">
+        <v>1.253912026</v>
+      </c>
+      <c r="B1441" t="n">
+        <v>94951893</v>
+      </c>
+      <c r="C1441" t="n">
+        <v>418212727841</v>
+      </c>
+      <c r="D1441" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="E1441" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="F1441" t="inlineStr">
+        <is>
+          <t>WARRNAMBOOL</t>
+        </is>
+      </c>
+      <c r="G1441" t="inlineStr">
+        <is>
+          <t>R2</t>
+        </is>
+      </c>
+      <c r="H1441" t="inlineStr">
+        <is>
+          <t>IM TO BLAME</t>
+        </is>
+      </c>
+      <c r="I1441" t="inlineStr">
+        <is>
+          <t>LAY</t>
+        </is>
+      </c>
+      <c r="J1441" t="inlineStr">
+        <is>
+          <t>UNMATCHED</t>
+        </is>
+      </c>
+      <c r="K1441" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="L1441" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1441" t="n">
+        <v>30</v>
+      </c>
+      <c r="N1441" t="inlineStr">
+        <is>
+          <t>LOSER</t>
+        </is>
+      </c>
+      <c r="O1441" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="n">
+        <v>1.253912026</v>
+      </c>
+      <c r="B1442" t="inlineStr"/>
+      <c r="C1442" t="inlineStr"/>
+      <c r="D1442" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="E1442" t="inlineStr"/>
+      <c r="F1442" t="inlineStr"/>
+      <c r="G1442" t="inlineStr"/>
+      <c r="H1442" t="inlineStr">
+        <is>
+          <t>IM TO BLAME</t>
+        </is>
+      </c>
+      <c r="I1442" t="inlineStr">
+        <is>
+          <t>LAY</t>
+        </is>
+      </c>
+      <c r="J1442" t="inlineStr">
+        <is>
+          <t>CAP_EXIT</t>
+        </is>
+      </c>
+      <c r="K1442" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1442" t="inlineStr"/>
+      <c r="M1442" t="inlineStr"/>
+      <c r="N1442" t="inlineStr"/>
+      <c r="O1442" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="n">
+        <v>1.253916374</v>
+      </c>
+      <c r="B1443" t="n">
+        <v>94410388</v>
+      </c>
+      <c r="C1443" t="n">
+        <v>418216966751</v>
+      </c>
+      <c r="D1443" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="E1443" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="F1443" t="inlineStr">
+        <is>
+          <t>SANDOWN PARK</t>
+        </is>
+      </c>
+      <c r="G1443" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="H1443" t="inlineStr">
+        <is>
+          <t>TONY</t>
+        </is>
+      </c>
+      <c r="I1443" t="inlineStr">
+        <is>
+          <t>LAY</t>
+        </is>
+      </c>
+      <c r="J1443" t="inlineStr">
+        <is>
+          <t>SETTLED</t>
+        </is>
+      </c>
+      <c r="K1443" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="L1443" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="M1443" t="n">
+        <v>10.7776555258094</v>
+      </c>
+      <c r="N1443" t="inlineStr">
+        <is>
+          <t>WIN</t>
+        </is>
+      </c>
+      <c r="O1443" t="n">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="n">
+        <v>1.253913347</v>
+      </c>
+      <c r="B1444" t="n">
+        <v>94922671</v>
+      </c>
+      <c r="C1444" t="n">
+        <v>418226097324</v>
+      </c>
+      <c r="D1444" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="E1444" t="inlineStr">
+        <is>
+          <t>22:44</t>
+        </is>
+      </c>
+      <c r="F1444" t="inlineStr">
+        <is>
+          <t>CASINO</t>
+        </is>
+      </c>
+      <c r="G1444" t="inlineStr">
+        <is>
+          <t>R12</t>
+        </is>
+      </c>
+      <c r="H1444" t="inlineStr">
+        <is>
+          <t>TIGGY BOODIE</t>
+        </is>
+      </c>
+      <c r="I1444" t="inlineStr">
+        <is>
+          <t>LAY</t>
+        </is>
+      </c>
+      <c r="J1444" t="inlineStr">
+        <is>
+          <t>SETTLED</t>
+        </is>
+      </c>
+      <c r="K1444" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="L1444" t="n">
+        <v>12</v>
+      </c>
+      <c r="M1444" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="N1444" t="inlineStr">
+        <is>
+          <t>WIN</t>
+        </is>
+      </c>
+      <c r="O1444" t="n">
+        <v>0.8400000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -82891,7 +83170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -85385,6 +85664,73 @@
       <c r="O37" t="inlineStr">
         <is>
           <t>96.3%</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="n">
+        <v>46065</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>$1.86</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>$1.71</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>91.9%</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>$0.00</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="L38" t="n">
+        <v>2</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>$1.71</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>91.9%</t>
         </is>
       </c>
     </row>
@@ -85891,10 +86237,10 @@
         <v>46062</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -85903,17 +86249,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$1.88</t>
+          <t>$3.74</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$1.81</t>
+          <t>$3.52</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>96.3%</t>
+          <t>94.1%</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -85935,7 +86281,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -85944,12 +86290,12 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>$1.81</t>
+          <t>$3.52</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>96.3%</t>
+          <t>94.1%</t>
         </is>
       </c>
     </row>
@@ -86121,29 +86467,29 @@
         <v>46054</v>
       </c>
       <c r="B3" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C3" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>68.8%</t>
+          <t>69.5%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$149.76</t>
+          <t>$151.62</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$-31.95</t>
+          <t>$-30.24</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-21.3%</t>
+          <t>-19.9%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -86165,21 +86511,21 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>80.9%</t>
+          <t>81.4%</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>$-28.50</t>
+          <t>$-26.79</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>-19.5%</t>
+          <t>-18.1%</t>
         </is>
       </c>
     </row>
@@ -86281,29 +86627,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C2" t="n">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>79.8%</t>
+          <t>79.9%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>$675.51</t>
+          <t>$677.37</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$-135.94</t>
+          <t>$-134.23</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-20.1%</t>
+          <t>-19.8%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -86325,7 +86671,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -86334,12 +86680,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>$-127.94</t>
+          <t>$-126.23</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>-19.4%</t>
+          <t>-19.1%</t>
         </is>
       </c>
     </row>

</xml_diff>